<commit_message>
Casos de Prueba v1.0
</commit_message>
<xml_diff>
--- a/Desarrollo/BiblioTech/documentacion/Casos de Prueba.xlsx
+++ b/Desarrollo/BiblioTech/documentacion/Casos de Prueba.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HOLA MUNDO\Desktop\FISI 2021-1\GESTION\GRUPAL\enPROCESO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HOLA MUNDO\Desktop\FISI 2021-1\GESTION\GRUPAL\pClonar\CGNSTECH\Desarrollo\BiblioTech\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Nomenclatura" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1.Casos de Prueba '!$B$9:$D$20</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1.Casos de Prueba '!$B$9:$D$19</definedName>
     <definedName name="Complejidad">#REF!</definedName>
     <definedName name="ESTADOS">Nomenclatura!$B$3:$B$7</definedName>
     <definedName name="Flujo">#REF!</definedName>
@@ -581,6 +581,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -597,7 +598,6 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -817,10 +817,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J928"/>
+  <dimension ref="A1:J927"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -835,45 +835,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="24"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
+      <c r="A2" s="25"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
     </row>
     <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="24"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
+      <c r="A3" s="25"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
     </row>
     <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E4" s="18"/>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="23" t="s">
         <v>53</v>
       </c>
       <c r="B5" s="18" t="s">
@@ -882,7 +882,7 @@
       <c r="E5" s="18"/>
     </row>
     <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="23" t="s">
         <v>54</v>
       </c>
       <c r="E6" s="18"/>
@@ -891,19 +891,19 @@
       <c r="E7" s="18"/>
     </row>
     <row r="8" spans="1:9" s="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="23" t="s">
+      <c r="B8" s="27"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="I8" s="23" t="s">
+      <c r="I8" s="24" t="s">
         <v>18</v>
       </c>
     </row>
@@ -929,8 +929,8 @@
       <c r="G9" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
     </row>
     <row r="10" spans="1:9" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11"/>
@@ -959,7 +959,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A11" s="11"/>
       <c r="B11" s="12" t="s">
         <v>41</v>
@@ -986,7 +986,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A12" s="11"/>
       <c r="B12" s="12" t="s">
         <v>41</v>
@@ -1155,29 +1155,19 @@
       <c r="I19" s="16"/>
     </row>
     <row r="20" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A20" s="11"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="16"/>
-      <c r="I20" s="16"/>
-    </row>
-    <row r="21" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="H21" s="17"/>
-      <c r="I21" s="17"/>
-    </row>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17"/>
+    </row>
+    <row r="21" spans="1:10" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="22" spans="1:10" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="23" spans="1:10" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="J24" s="21"/>
-    </row>
+    <row r="23" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="J23" s="21"/>
+    </row>
+    <row r="24" spans="1:10" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="25" spans="1:10" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="26" spans="1:10" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="27" spans="1:10" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:10" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1314,9 +1304,8 @@
     <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <autoFilter ref="B9:D20"/>
+  <autoFilter ref="B9:D19"/>
   <mergeCells count="4">
     <mergeCell ref="H8:H9"/>
     <mergeCell ref="I8:I9"/>
@@ -1333,13 +1322,13 @@
           <x14:formula1>
             <xm:f>Nomenclatura!$B$4:$B$9</xm:f>
           </x14:formula1>
-          <xm:sqref>H10:H20</xm:sqref>
+          <xm:sqref>H10:H19</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Nomenclatura!$F$4:$F$10</xm:f>
           </x14:formula1>
-          <xm:sqref>G10:G20</xm:sqref>
+          <xm:sqref>G10:G19</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>